<commit_message>
Replaced xlsx library with readxl to renove rJava requirement and did some minor editing
</commit_message>
<xml_diff>
--- a/code/data/population.xlsx
+++ b/code/data/population.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3340" yWindow="500" windowWidth="25600" windowHeight="14260" tabRatio="500"/>
+    <workbookView xWindow="3345" yWindow="495" windowWidth="25605" windowHeight="14265" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -89,6 +93,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -417,12 +426,12 @@
   <dimension ref="A1:KQ12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:303">
+    <row r="1" spans="1:303" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>129889</v>
       </c>
@@ -1333,7 +1342,7 @@
         <v>2297</v>
       </c>
     </row>
-    <row r="2" spans="1:303">
+    <row r="2" spans="1:303" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>127051</v>
       </c>
@@ -2244,7 +2253,7 @@
         <v>2376</v>
       </c>
     </row>
-    <row r="3" spans="1:303">
+    <row r="3" spans="1:303" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>127145</v>
       </c>
@@ -3155,7 +3164,7 @@
         <v>2386</v>
       </c>
     </row>
-    <row r="4" spans="1:303">
+    <row r="4" spans="1:303" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>129043</v>
       </c>
@@ -4066,7 +4075,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="5" spans="1:303">
+    <row r="5" spans="1:303" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>132634</v>
       </c>
@@ -4977,7 +4986,7 @@
         <v>2434</v>
       </c>
     </row>
-    <row r="6" spans="1:303">
+    <row r="6" spans="1:303" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>138322</v>
       </c>
@@ -5888,7 +5897,7 @@
         <v>2440</v>
       </c>
     </row>
-    <row r="7" spans="1:303">
+    <row r="7" spans="1:303" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>141804</v>
       </c>
@@ -6799,7 +6808,7 @@
         <v>2607</v>
       </c>
     </row>
-    <row r="8" spans="1:303">
+    <row r="8" spans="1:303" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>147232</v>
       </c>
@@ -7710,7 +7719,7 @@
         <v>2742</v>
       </c>
     </row>
-    <row r="9" spans="1:303">
+    <row r="9" spans="1:303" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>151307</v>
       </c>
@@ -8621,7 +8630,7 @@
         <v>2770</v>
       </c>
     </row>
-    <row r="10" spans="1:303">
+    <row r="10" spans="1:303" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>148336</v>
       </c>
@@ -9532,7 +9541,7 @@
         <v>2907</v>
       </c>
     </row>
-    <row r="11" spans="1:303">
+    <row r="11" spans="1:303" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>150266</v>
       </c>
@@ -10443,7 +10452,7 @@
         <v>3049</v>
       </c>
     </row>
-    <row r="12" spans="1:303">
+    <row r="12" spans="1:303" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>152661</v>
       </c>

</xml_diff>